<commit_message>
Le coup de polish
</commit_message>
<xml_diff>
--- a/cauchemarhouse/manuel/voca cauchemar.xlsx
+++ b/cauchemarhouse/manuel/voca cauchemar.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/antoine/Documents/antoine/apple iigs/crossdevtools/source/cauchemarhouse/manuel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FC2FD10A-2AA1-EB4A-B73C-08C0B3F84A55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F0E0E43-3124-CC42-BC21-9AEDF2537DB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{65A22FE6-8C59-6C4C-99A4-57696E5EF76B}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="96">
   <si>
     <t>NORTH</t>
   </si>
@@ -314,6 +314,15 @@
   </si>
   <si>
     <t>CASSE*</t>
+  </si>
+  <si>
+    <t>ENTER</t>
+  </si>
+  <si>
+    <t>CASE*</t>
+  </si>
+  <si>
+    <t>QUIT*</t>
   </si>
 </sst>
 </file>
@@ -667,8 +676,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{106D0861-CE86-4E4A-9A2E-013614011FB5}">
   <dimension ref="A1:E50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E50"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C50" sqref="C1:C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -817,7 +826,7 @@
         <v>CASE</v>
       </c>
       <c r="C10" t="s">
-        <v>45</v>
+        <v>94</v>
       </c>
       <c r="E10" t="s">
         <v>57</v>
@@ -936,7 +945,7 @@
         <v>46</v>
       </c>
       <c r="C18" t="s">
-        <v>46</v>
+        <v>93</v>
       </c>
       <c r="E18" t="s">
         <v>85</v>
@@ -981,7 +990,7 @@
         <v>GO</v>
       </c>
       <c r="C21" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="E21" t="s">
         <v>67</v>
@@ -996,7 +1005,7 @@
         <v>GUN</v>
       </c>
       <c r="C22" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="E22" t="s">
         <v>80</v>
@@ -1011,7 +1020,7 @@
         <v>HIT</v>
       </c>
       <c r="C23" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="E23" t="s">
         <v>68</v>
@@ -1026,7 +1035,7 @@
         <v>INSERT</v>
       </c>
       <c r="C24" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="E24" t="s">
         <v>61</v>
@@ -1041,7 +1050,7 @@
         <v>INVE</v>
       </c>
       <c r="C25" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="E25" t="s">
         <v>82</v>
@@ -1056,7 +1065,7 @@
         <v>KKKK</v>
       </c>
       <c r="C26" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E26" t="s">
         <v>21</v>
@@ -1071,7 +1080,7 @@
         <v>LAMP</v>
       </c>
       <c r="C27" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E27" t="s">
         <v>73</v>
@@ -1085,7 +1094,7 @@
         <v>47</v>
       </c>
       <c r="C28" t="s">
-        <v>47</v>
+        <v>13</v>
       </c>
       <c r="E28" t="s">
         <v>84</v>
@@ -1100,7 +1109,7 @@
         <v>LIGHT</v>
       </c>
       <c r="C29" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="E29" t="s">
         <v>75</v>
@@ -1115,7 +1124,7 @@
         <v>LOOK</v>
       </c>
       <c r="C30" t="s">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="E30" t="s">
         <v>74</v>
@@ -1130,7 +1139,7 @@
         <v>MOTE</v>
       </c>
       <c r="C31" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="E31" t="s">
         <v>32</v>
@@ -1145,7 +1154,7 @@
         <v>NORTH</v>
       </c>
       <c r="C32" t="s">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="E32" t="s">
         <v>51</v>
@@ -1160,7 +1169,7 @@
         <v>NOTHING</v>
       </c>
       <c r="C33" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E33" t="s">
         <v>78</v>
@@ -1175,7 +1184,7 @@
         <v>ORQU</v>
       </c>
       <c r="C34" t="s">
-        <v>33</v>
+        <v>5</v>
       </c>
       <c r="E34" t="s">
         <v>33</v>
@@ -1190,7 +1199,7 @@
         <v>PLUG</v>
       </c>
       <c r="C35" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E35" t="s">
         <v>52</v>
@@ -1205,7 +1214,7 @@
         <v>PULL</v>
       </c>
       <c r="C36" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E36" t="s">
         <v>71</v>
@@ -1220,7 +1229,7 @@
         <v>PUSH</v>
       </c>
       <c r="C37" t="s">
-        <v>8</v>
+        <v>95</v>
       </c>
       <c r="E37" t="s">
         <v>70</v>
@@ -1235,7 +1244,7 @@
         <v>PUSH</v>
       </c>
       <c r="C38" t="s">
-        <v>8</v>
+        <v>47</v>
       </c>
       <c r="E38" t="s">
         <v>83</v>
@@ -1250,7 +1259,7 @@
         <v>QUIT</v>
       </c>
       <c r="C39" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="E39" t="s">
         <v>88</v>
@@ -1265,7 +1274,7 @@
         <v>REPA</v>
       </c>
       <c r="C40" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="E40" t="s">
         <v>66</v>
@@ -1280,7 +1289,7 @@
         <v>SOCKET</v>
       </c>
       <c r="C41" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E41" t="s">
         <v>58</v>
@@ -1295,7 +1304,7 @@
         <v>SOUTH</v>
       </c>
       <c r="C42" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="E42" t="s">
         <v>91</v>
@@ -1310,7 +1319,7 @@
         <v>STICK</v>
       </c>
       <c r="C43" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="E43" t="s">
         <v>81</v>
@@ -1325,7 +1334,7 @@
         <v>SUIT</v>
       </c>
       <c r="C44" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="E44" t="s">
         <v>63</v>
@@ -1355,7 +1364,7 @@
         <v>TEMPO</v>
       </c>
       <c r="C46" t="s">
-        <v>43</v>
+        <v>90</v>
       </c>
       <c r="E46" t="s">
         <v>79</v>
@@ -1422,8 +1431,8 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="E1:E50">
-    <sortCondition ref="E1:E50"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C1:C50">
+    <sortCondition ref="C1:C50"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>